<commit_message>
experiment with alternate model specs for rhme
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -359,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,175 +379,175 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>130</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>130</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>130</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>130</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>130</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>130</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>130</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>130</v>
@@ -611,9 +611,17 @@
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>130</v>
       </c>
     </row>
@@ -624,7 +632,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -644,199 +652,199 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>130</v>
@@ -844,7 +852,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>130</v>
@@ -852,7 +860,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>130</v>
@@ -860,7 +868,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>130</v>
@@ -868,7 +876,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>130</v>
@@ -876,9 +884,17 @@
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>130</v>
       </c>
     </row>
@@ -889,7 +905,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -909,215 +925,215 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>130</v>
@@ -1125,7 +1141,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>130</v>
@@ -1133,7 +1149,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>130</v>
@@ -1141,9 +1157,17 @@
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>130</v>
       </c>
     </row>
@@ -1154,7 +1178,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1174,241 +1198,249 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>130</v>
       </c>
     </row>
@@ -1419,7 +1451,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1439,241 +1471,249 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>127</v>
       </c>
     </row>
@@ -1684,7 +1724,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1704,241 +1744,249 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>123</v>
       </c>
     </row>
@@ -1949,7 +1997,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1969,241 +2017,249 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>123</v>
       </c>
     </row>
@@ -2214,7 +2270,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2234,241 +2290,249 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>123</v>
       </c>
     </row>
@@ -2479,7 +2543,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2499,242 +2563,250 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>109</v>
+      <c r="B32">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun tode norms thru rhme
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -382,7 +382,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4">
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
@@ -430,7 +430,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10">
@@ -446,7 +446,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
@@ -454,7 +454,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -470,7 +470,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15">
@@ -486,7 +486,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16">
@@ -526,7 +526,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21">
@@ -534,7 +534,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22">
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23">
@@ -655,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
@@ -687,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
@@ -695,7 +695,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +703,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
@@ -727,7 +727,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13">
@@ -743,7 +743,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
@@ -751,7 +751,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17">
@@ -807,7 +807,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22">
@@ -815,7 +815,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23">
@@ -823,7 +823,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24">
@@ -831,7 +831,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
@@ -839,7 +839,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26">
@@ -847,7 +847,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27">
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -944,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -960,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
@@ -968,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
@@ -976,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -984,7 +984,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
@@ -992,7 +992,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
@@ -1000,7 +1000,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -1008,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -1016,7 +1016,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -1024,7 +1024,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
@@ -1032,7 +1032,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16">
@@ -1048,7 +1048,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18">
@@ -1080,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22">
@@ -1088,7 +1088,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23">
@@ -1096,7 +1096,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24">
@@ -1104,7 +1104,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25">
@@ -1112,7 +1112,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
@@ -1120,7 +1120,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
@@ -1128,7 +1128,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
@@ -1136,7 +1136,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
@@ -1144,7 +1144,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30">
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -1217,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -1225,7 +1225,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -1233,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -1241,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
@@ -1249,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
@@ -1257,7 +1257,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10">
@@ -1265,7 +1265,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -1273,7 +1273,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12">
@@ -1281,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13">
@@ -1289,7 +1289,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
@@ -1297,7 +1297,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
@@ -1313,7 +1313,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17">
@@ -1345,7 +1345,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -1353,7 +1353,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
@@ -1361,7 +1361,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -1369,7 +1369,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24">
@@ -1377,7 +1377,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -1385,7 +1385,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -1393,7 +1393,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
@@ -1401,7 +1401,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -1409,7 +1409,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -1417,7 +1417,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -1425,7 +1425,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
@@ -1433,7 +1433,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -1482,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
@@ -1490,7 +1490,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
@@ -1498,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -1506,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -1514,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
@@ -1530,7 +1530,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
@@ -1538,7 +1538,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
@@ -1546,7 +1546,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
@@ -1554,7 +1554,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
@@ -1562,7 +1562,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14">
@@ -1570,7 +1570,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -1578,7 +1578,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
@@ -1586,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
@@ -1626,7 +1626,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -1634,7 +1634,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
@@ -1642,7 +1642,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -1650,7 +1650,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
@@ -1658,7 +1658,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
@@ -1666,7 +1666,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -1674,7 +1674,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
@@ -1682,7 +1682,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29">
@@ -1690,7 +1690,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30">
@@ -1698,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -1714,7 +1714,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -1763,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -1771,7 +1771,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -1779,7 +1779,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -1787,7 +1787,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -1795,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
@@ -1803,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10">
@@ -1811,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
@@ -1819,7 +1819,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12">
@@ -1827,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
@@ -1835,7 +1835,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
@@ -1843,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -1851,7 +1851,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -1867,7 +1867,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -1891,7 +1891,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1899,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -1907,7 +1907,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
@@ -1915,7 +1915,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -1923,7 +1923,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
@@ -1931,7 +1931,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26">
@@ -1939,7 +1939,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -1947,7 +1947,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -1955,7 +1955,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -1963,7 +1963,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -1971,7 +1971,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
@@ -1979,7 +1979,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
@@ -1987,7 +1987,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
@@ -2028,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -2036,7 +2036,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -2044,7 +2044,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
@@ -2052,7 +2052,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -2060,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -2068,7 +2068,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
@@ -2076,7 +2076,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10">
@@ -2084,7 +2084,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -2092,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
@@ -2100,7 +2100,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -2108,7 +2108,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -2116,7 +2116,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -2124,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -2132,7 +2132,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -2172,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
@@ -2180,7 +2180,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -2188,7 +2188,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
@@ -2196,7 +2196,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25">
@@ -2204,7 +2204,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -2212,7 +2212,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -2220,7 +2220,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
@@ -2228,7 +2228,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29">
@@ -2236,7 +2236,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -2244,7 +2244,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31">
@@ -2252,7 +2252,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
@@ -2260,7 +2260,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
@@ -2309,7 +2309,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
@@ -2317,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -2325,7 +2325,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
@@ -2333,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
@@ -2341,7 +2341,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -2349,7 +2349,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -2357,7 +2357,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -2365,7 +2365,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -2373,7 +2373,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -2381,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -2389,7 +2389,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -2397,7 +2397,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -2405,7 +2405,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -2453,7 +2453,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
@@ -2461,7 +2461,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
@@ -2469,7 +2469,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
@@ -2493,7 +2493,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28">
@@ -2501,7 +2501,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29">
@@ -2509,7 +2509,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30">
@@ -2517,7 +2517,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -2525,7 +2525,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32">
@@ -2566,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -2582,7 +2582,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -2590,7 +2590,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -2598,7 +2598,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -2606,7 +2606,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -2614,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -2622,7 +2622,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
@@ -2630,7 +2630,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -2638,7 +2638,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
@@ -2646,7 +2646,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
@@ -2654,7 +2654,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -2662,7 +2662,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -2670,7 +2670,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -2678,7 +2678,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -2686,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -2694,7 +2694,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
@@ -2702,7 +2702,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
@@ -2726,7 +2726,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -2734,7 +2734,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
@@ -2742,7 +2742,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
@@ -2750,7 +2750,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -2758,7 +2758,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -2766,7 +2766,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
@@ -2774,7 +2774,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29">
@@ -2782,7 +2782,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30">
@@ -2790,7 +2790,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31">
@@ -2798,7 +2798,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32">
@@ -2806,7 +2806,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>